<commit_message>
update lista de sku
</commit_message>
<xml_diff>
--- a/sku.xlsx
+++ b/sku.xlsx
@@ -1,35 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dato\OneDrive\Documentos\Datoo\REPOSITÓRIOS\python\shelflife\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dato\Dropbox\Amplo 2024\2- Projetos Amplo 2024\PAPAPA\CONTROLE SHELFLIFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3B622C-7ACB-4B9A-9622-85BEEFEA7FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07593D72-ABA0-4F67-88D8-CC508042DB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp_url_15_ambiente_141_user_9" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>7898994908739/AMOSTRA</t>
-  </si>
-  <si>
-    <t>7898994908746/AMOSTRA</t>
-  </si>
-  <si>
-    <t>7898994908753/AMOSTRA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>TESTESHELFLIFE</t>
   </si>
@@ -41,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,9 +181,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <b/>
+      <sz val="16"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="OpenSansRegular"/>
     </font>
   </fonts>
   <fills count="33">
@@ -538,17 +548,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -609,9 +621,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -649,7 +661,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -755,7 +767,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -897,7 +909,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -905,110 +917,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="H11" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="21">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4">
         <v>7898994908722</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="3" spans="1:1">
+      <c r="A3" s="4">
         <v>7898994908739</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="4" spans="1:1">
+      <c r="A4" s="4">
         <v>7898994908746</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="5" spans="1:1">
+      <c r="A5" s="4">
         <v>7898994908753</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+    <row r="6" spans="1:1">
+      <c r="A6" s="4">
         <v>7898994908715</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="4">
+        <v>8777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="4">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="4">
+        <v>5071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="4">
+        <v>5088</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="4">
+        <v>8760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>8777</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>6065</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>5064</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>5071</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>5088</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>8760</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3">
+    <row r="13" spans="1:1">
+      <c r="A13" s="4">
         <v>7896579902028</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
+    <row r="14" spans="1:1">
+      <c r="A14" s="4">
         <v>5293</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3">
+    <row r="15" spans="1:1">
+      <c r="A15" s="4">
         <v>5286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="4">
+        <v>5255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4">
+        <v>5279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="4">
+        <v>5262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="4">
+        <v>3342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="4">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="4">
+        <v>5354</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="4">
+        <v>5361</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="4">
+        <v>5378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="4">
+        <v>5309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="4">
+        <v>5316</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="5">
+        <v>5323</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="6">
+        <v>5378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>